<commit_message>
Completei a primeira tabela e mudei nn_train para fazer a media dos 10 automaticamente
</commit_message>
<xml_diff>
--- a/estudoNN_TP.xlsx
+++ b/estudoNN_TP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://isecpt-my.sharepoint.com/personal/a2020131717_isec_pt/Documents/ISEC/2º Ano/2º Semestre/CR/CR-GrupoTrabalhoPratico/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Downloads\CR-GrupoTrabalhoPratico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{44F9B90B-6E82-F445-B223-3A65CE2FC243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{117DB123-EB3F-45B3-B56D-BC8F7E8390BA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945BA733-49E9-47FC-9B9E-C80D6BA81DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IRIS" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
   <si>
     <t>Função de treino</t>
   </si>
@@ -120,22 +120,19 @@
     <t>trainlm</t>
   </si>
   <si>
-    <t>99.43</t>
-  </si>
-  <si>
-    <t>98.69</t>
-  </si>
-  <si>
-    <t>97.45</t>
-  </si>
-  <si>
-    <t>95.56</t>
-  </si>
-  <si>
     <t>97.84</t>
   </si>
   <si>
     <t>96.67</t>
+  </si>
+  <si>
+    <t>5,10,5</t>
+  </si>
+  <si>
+    <t>tansig, tansig,tansig, purelin</t>
+  </si>
+  <si>
+    <t>10,10,10</t>
   </si>
 </sst>
 </file>
@@ -789,20 +786,20 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.75" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.69921875" customWidth="1"/>
+    <col min="7" max="7" width="5.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -826,8 +823,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="46.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="46.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -848,15 +845,15 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:9" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
@@ -869,7 +866,7 @@
       <c r="H6" s="10"/>
       <c r="I6" s="11"/>
     </row>
-    <row r="7" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -889,14 +886,14 @@
         <v>11</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H7" s="4">
+        <v>98.89</v>
+      </c>
+      <c r="I7" s="5">
+        <v>97.88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -916,21 +913,25 @@
         <v>11</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="4">
+        <v>99.26</v>
+      </c>
+      <c r="I8" s="5">
+        <v>97.89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="6">
+        <v>3</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="D9" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>29</v>
@@ -939,17 +940,25 @@
         <v>11</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H9" s="4">
+        <v>98.78</v>
+      </c>
+      <c r="I9" s="5">
+        <v>96.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="6">
+        <v>3</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="D10" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>29</v>
@@ -958,11 +967,15 @@
         <v>11</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:9" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H10" s="4">
+        <v>98.834000000000003</v>
+      </c>
+      <c r="I10" s="5">
+        <v>96.61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:9" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
@@ -975,7 +988,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="11"/>
     </row>
-    <row r="13" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -998,7 +1011,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1021,7 +1034,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1042,7 +1055,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1063,8 +1076,8 @@
       <c r="H16" s="4"/>
       <c r="I16" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:9" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:9" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>23</v>
       </c>
@@ -1077,7 +1090,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -1100,7 +1113,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1123,7 +1136,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -1144,7 +1157,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
@@ -1165,7 +1178,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1186,7 +1199,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -1207,8 +1220,8 @@
       <c r="H25" s="4"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:9" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:9" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>22</v>
       </c>
@@ -1221,7 +1234,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
@@ -1244,7 +1257,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1267,7 +1280,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -1280,7 +1293,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
@@ -1293,7 +1306,7 @@
       <c r="H31" s="4"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1306,7 +1319,7 @@
       <c r="H32" s="4"/>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:9" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Completei o excel do estudos do dataset train 3.4b) e mudei nn_train.m para medir tambem o tempo de teste
</commit_message>
<xml_diff>
--- a/estudoNN_TP.xlsx
+++ b/estudoNN_TP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Downloads\CR-GrupoTrabalhoPratico\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Documents\isec\CR\CR-GrupoTrabalhoPratico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945BA733-49E9-47FC-9B9E-C80D6BA81DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C9EE02-87B0-4E05-8C76-8109C7CE6BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="106">
   <si>
     <t>Função de treino</t>
   </si>
@@ -133,6 +133,244 @@
   </si>
   <si>
     <t>10,10,10</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>93.47</t>
+  </si>
+  <si>
+    <t>93.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 93.15</t>
+  </si>
+  <si>
+    <t>99.44</t>
+  </si>
+  <si>
+    <t>98.93</t>
+  </si>
+  <si>
+    <t>99.26</t>
+  </si>
+  <si>
+    <t>98.48</t>
+  </si>
+  <si>
+    <t>99.43</t>
+  </si>
+  <si>
+    <t>99.09</t>
+  </si>
+  <si>
+    <t>99.53</t>
+  </si>
+  <si>
+    <t>98.50</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.002
+Media de tempo para o teste: 0.005</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.004
+Media de tempo para o teste: 0.01</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.005
+Media de tempo para o teste: 0.009</t>
+  </si>
+  <si>
+    <t>Foi o que obteve melhor resultados devido ao aumento de neuronios e camadas
+Media de tempo para o treino: 0.002
+Media de tempo para o teste: 0.01</t>
+  </si>
+  <si>
+    <t>Ao aumentar o numeros de neuronios e camadas consegue melhor precisão</t>
+  </si>
+  <si>
+    <t>98.91</t>
+  </si>
+  <si>
+    <t>98.77</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.010811
+Media de tempo para o teste: 0.012303</t>
+  </si>
+  <si>
+    <t>traingdm</t>
+  </si>
+  <si>
+    <t>Diferente das outras funções treino esta chega fazer todas epochs chegandos as 1000
+Media de tempo para o treino: 0.064817
+Media de tempo para o teste: 0.068498</t>
+  </si>
+  <si>
+    <t>trainscg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esta função tambem faz ate 1000 epochs diferente da trainbfg e trainscg
+Media de tempo para o treino: 0.06
+Media de tempo para o teste: 0.06 </t>
+  </si>
+  <si>
+    <t>97.89</t>
+  </si>
+  <si>
+    <t>98.03</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.021170
+Media de tempo para o teste: 0.019692</t>
+  </si>
+  <si>
+    <t>Ao mudar a função de treino obtem se pior precisao global comparado a função "trainml"
+ e tambem demoram mais tempo a treinar.
+Tambem vi que traingd e traingdm vao ate as 1000 epcohs enquanto outra fazem por volta de 6-30 epochs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 98.94</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.003962
+Media de tempo para o teste: 0.010624</t>
+  </si>
+  <si>
+    <t>99.25</t>
+  </si>
+  <si>
+    <t>98.65</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.006623
+Media de tempo para o teste: 0.013495</t>
+  </si>
+  <si>
+    <t>compet,ellistig</t>
+  </si>
+  <si>
+    <t>79.52</t>
+  </si>
+  <si>
+    <t>78.04</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.201231
+Media de tempo para o teste: 0.219569</t>
+  </si>
+  <si>
+    <t>hardlims,hardlim</t>
+  </si>
+  <si>
+    <t>71.68</t>
+  </si>
+  <si>
+    <t>72.84</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.284576
+Media de tempo para o teste: 0.271552</t>
+  </si>
+  <si>
+    <t>compet,logsig</t>
+  </si>
+  <si>
+    <t>77.30</t>
+  </si>
+  <si>
+    <t>77.55</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.226114
+Media de tempo para o teste: 0.224481</t>
+  </si>
+  <si>
+    <t>hardlim,hardlims</t>
+  </si>
+  <si>
+    <t>40.66</t>
+  </si>
+  <si>
+    <t>42.07</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.597248
+Media de tempo para o teste: 0.579310</t>
+  </si>
+  <si>
+    <t>98.88</t>
+  </si>
+  <si>
+    <t>98.28</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.007156
+Media de tempo para o teste: 0.017219</t>
+  </si>
+  <si>
+    <t>99.67</t>
+  </si>
+  <si>
+    <t>99.99</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.003326
+Media de tempo para o teste: 0.000082</t>
+  </si>
+  <si>
+    <t>dividerand = {0.8, 0.10, 0.10}</t>
+  </si>
+  <si>
+    <t>dividerand = {0.1, 0.80, 0.10}</t>
+  </si>
+  <si>
+    <t>99.60</t>
+  </si>
+  <si>
+    <t>99.56</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.004227
+Media de tempo para o teste: 0.004412</t>
+  </si>
+  <si>
+    <t>96.48</t>
+  </si>
+  <si>
+    <t>96.88</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.023621
+Media de tempo para o teste: 0.031246</t>
+  </si>
+  <si>
+    <t>dividerand = {0.6, 0.20, 0.20}</t>
+  </si>
+  <si>
+    <t>dividerand = {0.4, 0.20, 0.40}</t>
+  </si>
+  <si>
+    <t>98.81</t>
+  </si>
+  <si>
+    <t>98.39</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.010795
+Media de tempo para o teste: 0.016056</t>
+  </si>
+  <si>
+    <t>99.06</t>
+  </si>
+  <si>
+    <t>98.63</t>
+  </si>
+  <si>
+    <t>Media de tempo para o treino: 0.004080
+Media de tempo para o teste: 0.013671</t>
   </si>
 </sst>
 </file>
@@ -216,7 +454,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -261,6 +499,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -337,7 +584,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -363,6 +610,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -371,6 +622,19 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="73">
@@ -783,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35:J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -799,7 +1063,7 @@
     <col min="7" max="7" width="5.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -822,9 +1086,18 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="46.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+    </row>
+    <row r="2" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:17" ht="46.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -850,23 +1123,41 @@
       <c r="I3" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:9" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="J3" s="16"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+    </row>
+    <row r="4" spans="1:17" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:17" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
-    </row>
-    <row r="7" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -886,14 +1177,24 @@
         <v>11</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="4">
-        <v>98.89</v>
-      </c>
-      <c r="I7" s="5">
-        <v>97.88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+    </row>
+    <row r="8" spans="1:17" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -913,14 +1214,24 @@
         <v>11</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="4">
-        <v>99.26</v>
-      </c>
-      <c r="I8" s="5">
-        <v>97.89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+    </row>
+    <row r="9" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -940,14 +1251,24 @@
         <v>11</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="4">
-        <v>98.78</v>
-      </c>
-      <c r="I9" s="5">
-        <v>96.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+    </row>
+    <row r="10" spans="1:17" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -967,28 +1288,48 @@
         <v>11</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="4">
-        <v>98.834000000000003</v>
-      </c>
-      <c r="I10" s="5">
-        <v>96.61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:9" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="H10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="11" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:17" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="11"/>
-    </row>
-    <row r="13" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+    </row>
+    <row r="13" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1008,10 +1349,23 @@
         <v>11</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1031,10 +1385,24 @@
         <v>11</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+    </row>
+    <row r="15" spans="1:17" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1047,15 +1415,31 @@
       <c r="D15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="F15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+    </row>
+    <row r="16" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1068,29 +1452,45 @@
       <c r="D16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="F16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:9" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="H16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+    </row>
+    <row r="18" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:17" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="20" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -1110,10 +1510,24 @@
         <v>11</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+    </row>
+    <row r="21" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1133,10 +1547,24 @@
         <v>11</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+    </row>
+    <row r="22" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -1146,7 +1574,9 @@
       <c r="C22" s="3">
         <v>10</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="E22" s="3" t="s">
         <v>29</v>
       </c>
@@ -1154,10 +1584,24 @@
         <v>11</v>
       </c>
       <c r="G22" s="3"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+    </row>
+    <row r="23" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
@@ -1167,7 +1611,9 @@
       <c r="C23" s="3">
         <v>10</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E23" s="3" t="s">
         <v>29</v>
       </c>
@@ -1175,10 +1621,24 @@
         <v>11</v>
       </c>
       <c r="G23" s="3"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+    </row>
+    <row r="24" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1188,7 +1648,9 @@
       <c r="C24" s="3">
         <v>10</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="E24" s="3" t="s">
         <v>29</v>
       </c>
@@ -1196,10 +1658,24 @@
         <v>11</v>
       </c>
       <c r="G24" s="3"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+    </row>
+    <row r="25" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -1209,7 +1685,9 @@
       <c r="C25" s="3">
         <v>10</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="E25" s="3" t="s">
         <v>29</v>
       </c>
@@ -1217,24 +1695,37 @@
         <v>11</v>
       </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:9" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
+      <c r="H25" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+    </row>
+    <row r="26" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:17" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="11"/>
-    </row>
-    <row r="28" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
@@ -1254,10 +1745,24 @@
         <v>27</v>
       </c>
       <c r="G28" s="3"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+    </row>
+    <row r="29" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1277,67 +1782,201 @@
         <v>28</v>
       </c>
       <c r="G29" s="3"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+    </row>
+    <row r="30" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3">
+        <v>10</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="G30" s="3"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H30" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+    </row>
+    <row r="31" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>10</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+    </row>
+    <row r="32" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3">
+        <v>10</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="G32" s="3"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H32" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+    </row>
+    <row r="33" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3">
+        <v>10</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="G33" s="3"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="5"/>
+      <c r="H33" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J33" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="28">
+    <mergeCell ref="J32:Q32"/>
+    <mergeCell ref="J33:Q33"/>
+    <mergeCell ref="J25:P25"/>
+    <mergeCell ref="J28:Q28"/>
+    <mergeCell ref="J29:Q29"/>
+    <mergeCell ref="J30:Q30"/>
+    <mergeCell ref="J31:Q31"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="J13:P13"/>
+    <mergeCell ref="J7:Q7"/>
+    <mergeCell ref="J8:Q8"/>
+    <mergeCell ref="J9:Q9"/>
+    <mergeCell ref="J10:Q10"/>
+    <mergeCell ref="J3:Q3"/>
+    <mergeCell ref="J6:Q6"/>
+    <mergeCell ref="J12:Q12"/>
+    <mergeCell ref="J14:Q14"/>
+    <mergeCell ref="J20:Q20"/>
+    <mergeCell ref="J21:Q21"/>
+    <mergeCell ref="J23:Q23"/>
+    <mergeCell ref="J22:Q22"/>
+    <mergeCell ref="J24:Q24"/>
+    <mergeCell ref="J15:Q15"/>
+    <mergeCell ref="J16:Q16"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A12:I12"/>
     <mergeCell ref="A19:I19"/>
-    <mergeCell ref="A27:I27"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Coluna ID / Conclusao da APP
A APP está concluida.
Fiz também o script da alinea c)
</commit_message>
<xml_diff>
--- a/estudoNN_TP.xlsx
+++ b/estudoNN_TP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://isecpt-my.sharepoint.com/personal/a2020131717_isec_pt/Documents/ISEC/2º Ano/2º Semestre/CR/CR-GrupoTrabalhoPratico/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{98C9EE02-87B0-4E05-8C76-8109C7CE6BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5AAA3EE-0710-478B-A616-796AED4AE76E}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{98C9EE02-87B0-4E05-8C76-8109C7CE6BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B203E77-AF0A-46AC-B856-155F7D71AD65}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23376" yWindow="9252" windowWidth="21600" windowHeight="11292" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IRIS" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="131">
   <si>
     <t>Função de treino</t>
   </si>
@@ -401,6 +401,51 @@
   </si>
   <si>
     <t>99.98</t>
+  </si>
+  <si>
+    <t>99.90</t>
+  </si>
+  <si>
+    <t>99.48</t>
+  </si>
+  <si>
+    <t>tansig, tansig, tansig, purelin</t>
+  </si>
+  <si>
+    <t>99.00</t>
+  </si>
+  <si>
+    <t>99.79</t>
+  </si>
+  <si>
+    <t>99.84</t>
+  </si>
+  <si>
+    <t>99.94</t>
+  </si>
+  <si>
+    <t>98.74</t>
+  </si>
+  <si>
+    <t>98.90</t>
+  </si>
+  <si>
+    <t>dividerand = {0.8, 0.1, 0.1}</t>
+  </si>
+  <si>
+    <t>99.76</t>
+  </si>
+  <si>
+    <t>99.69</t>
+  </si>
+  <si>
+    <t>99.87</t>
+  </si>
+  <si>
+    <t>99.75</t>
+  </si>
+  <si>
+    <t>99.57</t>
   </si>
 </sst>
 </file>
@@ -470,7 +515,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,6 +525,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,6 +697,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -650,6 +710,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -659,19 +726,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="73">
@@ -774,8 +833,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>501561</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>156399</xdr:rowOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>137349</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -809,6 +868,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1133,23 +1196,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q46"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.75" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.69921875" customWidth="1"/>
+    <col min="7" max="7" width="5.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1172,18 +1235,18 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-    </row>
-    <row r="2" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:17" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+    </row>
+    <row r="2" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:17" ht="46.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -1209,41 +1272,41 @@
       <c r="I3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-    </row>
-    <row r="4" spans="1:17" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:17" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="J3" s="16"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+    </row>
+    <row r="4" spans="1:17" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:17" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="18" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-    </row>
-    <row r="7" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="7" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1269,18 +1332,18 @@
       <c r="I7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-    </row>
-    <row r="8" spans="1:17" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:17" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1306,18 +1369,18 @@
       <c r="I8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-    </row>
-    <row r="9" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+    </row>
+    <row r="9" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1343,18 +1406,18 @@
       <c r="I9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-    </row>
-    <row r="10" spans="1:17" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+    </row>
+    <row r="10" spans="1:17" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1380,42 +1443,42 @@
       <c r="I10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-    </row>
-    <row r="11" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:17" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+    </row>
+    <row r="11" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:17" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="9" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-    </row>
-    <row r="13" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+    </row>
+    <row r="13" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1441,17 +1504,17 @@
       <c r="I13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-    </row>
-    <row r="14" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+    </row>
+    <row r="14" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1477,18 +1540,18 @@
       <c r="I14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-    </row>
-    <row r="15" spans="1:17" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+    </row>
+    <row r="15" spans="1:17" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1514,18 +1577,18 @@
       <c r="I15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-    </row>
-    <row r="16" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+    </row>
+    <row r="16" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1551,32 +1614,32 @@
       <c r="I16" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-    </row>
-    <row r="18" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:17" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13" t="s">
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+    </row>
+    <row r="18" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:17" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -1602,18 +1665,18 @@
       <c r="I20" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J20" s="9" t="s">
+      <c r="J20" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-    </row>
-    <row r="21" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+    </row>
+    <row r="21" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1639,18 +1702,18 @@
       <c r="I21" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="J21" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-    </row>
-    <row r="22" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+    </row>
+    <row r="22" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -1676,18 +1739,18 @@
       <c r="I22" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="J22" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-    </row>
-    <row r="23" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+    </row>
+    <row r="23" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
@@ -1713,18 +1776,18 @@
       <c r="I23" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J23" s="9" t="s">
+      <c r="J23" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-    </row>
-    <row r="24" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+    </row>
+    <row r="24" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1750,18 +1813,18 @@
       <c r="I24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="J24" s="9" t="s">
+      <c r="J24" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-    </row>
-    <row r="25" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+    </row>
+    <row r="25" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -1787,31 +1850,31 @@
       <c r="I25" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="J25" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-    </row>
-    <row r="26" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:17" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+    </row>
+    <row r="26" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:17" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="15"/>
-    </row>
-    <row r="28" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="19"/>
+    </row>
+    <row r="28" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
@@ -1837,18 +1900,18 @@
       <c r="I28" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J28" s="11" t="s">
+      <c r="J28" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-    </row>
-    <row r="29" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+    </row>
+    <row r="29" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1874,18 +1937,18 @@
       <c r="I29" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="J29" s="9" t="s">
+      <c r="J29" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-    </row>
-    <row r="30" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+    </row>
+    <row r="30" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -1911,18 +1974,18 @@
       <c r="I30" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J30" s="9" t="s">
+      <c r="J30" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-    </row>
-    <row r="31" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+    </row>
+    <row r="31" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
@@ -1948,18 +2011,18 @@
       <c r="I31" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="J31" s="9" t="s">
+      <c r="J31" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="10"/>
-    </row>
-    <row r="32" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+    </row>
+    <row r="32" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1985,18 +2048,18 @@
       <c r="I32" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="J32" s="9" t="s">
+      <c r="J32" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-    </row>
-    <row r="33" spans="1:17" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+    </row>
+    <row r="33" spans="1:17" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -2022,32 +2085,32 @@
       <c r="I33" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J33" s="11" t="s">
+      <c r="J33" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="12"/>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="12"/>
-    </row>
-    <row r="35" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="1:17" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="13" t="s">
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+    </row>
+    <row r="35" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="15"/>
-    </row>
-    <row r="37" spans="1:17" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="19"/>
+    </row>
+    <row r="37" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
@@ -2074,7 +2137,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>110</v>
       </c>
@@ -2087,7 +2150,7 @@
       <c r="D38" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="21" t="s">
+      <c r="E38" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F38" s="7" t="s">
@@ -2101,7 +2164,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>111</v>
       </c>
@@ -2128,7 +2191,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>112</v>
       </c>
@@ -2155,22 +2218,22 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="1:17" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="13" t="s">
+    <row r="44" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="15"/>
-    </row>
-    <row r="46" spans="1:17" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="19"/>
+    </row>
+    <row r="46" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="20" t="s">
         <v>113</v>
       </c>
       <c r="B46" s="6">
@@ -2194,6 +2257,223 @@
       </c>
       <c r="I46" s="5" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" s="6">
+        <v>3</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="6">
+        <v>3</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G48" s="3"/>
+      <c r="H48" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="6">
+        <v>3</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G49" s="3"/>
+      <c r="H49" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="6">
+        <v>3</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G50" s="3"/>
+      <c r="H50" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" s="6">
+        <v>3</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="H51" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="6">
+        <v>3</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="6">
+        <v>3</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G54" s="3"/>
+      <c r="H54" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" s="6">
+        <v>3</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="H55" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2206,6 +2486,14 @@
     <mergeCell ref="A12:I12"/>
     <mergeCell ref="A19:I19"/>
     <mergeCell ref="A27:I27"/>
+    <mergeCell ref="J14:Q14"/>
+    <mergeCell ref="J20:Q20"/>
+    <mergeCell ref="J21:Q21"/>
+    <mergeCell ref="J23:Q23"/>
+    <mergeCell ref="J22:Q22"/>
+    <mergeCell ref="J24:Q24"/>
+    <mergeCell ref="J32:Q32"/>
+    <mergeCell ref="J33:Q33"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="J13:P13"/>
     <mergeCell ref="J7:Q7"/>
@@ -2215,14 +2503,6 @@
     <mergeCell ref="J3:Q3"/>
     <mergeCell ref="J6:Q6"/>
     <mergeCell ref="J12:Q12"/>
-    <mergeCell ref="J14:Q14"/>
-    <mergeCell ref="J20:Q20"/>
-    <mergeCell ref="J21:Q21"/>
-    <mergeCell ref="J23:Q23"/>
-    <mergeCell ref="J22:Q22"/>
-    <mergeCell ref="J24:Q24"/>
-    <mergeCell ref="J32:Q32"/>
-    <mergeCell ref="J33:Q33"/>
     <mergeCell ref="J25:P25"/>
     <mergeCell ref="J28:Q28"/>
     <mergeCell ref="J29:Q29"/>

</xml_diff>

<commit_message>
Upgrade do Estudo Excel e remocao de ficheiros inuteis
</commit_message>
<xml_diff>
--- a/estudoNN_TP.xlsx
+++ b/estudoNN_TP.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://isecpt-my.sharepoint.com/personal/a2020131717_isec_pt/Documents/ISEC/2º Ano/2º Semestre/CR/CR-GrupoTrabalhoPratico/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1363" documentId="13_ncr:1_{98C9EE02-87B0-4E05-8C76-8109C7CE6BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F28C3CD1-697B-4E68-952D-1877097D95CD}"/>
+  <xr:revisionPtr revIDLastSave="1501" documentId="13_ncr:1_{98C9EE02-87B0-4E05-8C76-8109C7CE6BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABB059DE-75D1-43C7-9845-F20089F7ADD1}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="7488" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testes" sheetId="5" r:id="rId1"/>
     <sheet name="Resultados Ordenados" sheetId="7" r:id="rId2"/>
     <sheet name="TOP 3" sheetId="8" r:id="rId3"/>
+    <sheet name="Alinea C" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="258">
   <si>
     <t>Função de treino</t>
   </si>
@@ -799,13 +800,37 @@
   </si>
   <si>
     <t>best3.mat</t>
+  </si>
+  <si>
+    <t>Rede "best1.mat"</t>
+  </si>
+  <si>
+    <t>Rede "best3.mat"</t>
+  </si>
+  <si>
+    <t>Rede "best2.mat"</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Correto</t>
+  </si>
+  <si>
+    <t>Precisão = 60.00%</t>
+  </si>
+  <si>
+    <t>Precisão = 50.00%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -880,8 +905,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -918,8 +951,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1109,6 +1148,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1185,7 +1303,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1292,17 +1410,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="73">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8" hidden="1"/>
@@ -1379,7 +1569,38 @@
     <cellStyle name="Hiperligação Visitada" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1720,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6ED930A-590B-4292-AF26-736ED424ABED}">
   <dimension ref="B2:L69"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:L27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1805,30 +2026,30 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
     </row>
     <row r="6" spans="2:12" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="37" t="s">
@@ -3562,16 +3783,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B4:L5"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="B14:L15"/>
+    <mergeCell ref="B16:L16"/>
+    <mergeCell ref="B25:L26"/>
     <mergeCell ref="B27:L27"/>
     <mergeCell ref="B37:L38"/>
     <mergeCell ref="B39:L39"/>
     <mergeCell ref="B48:L49"/>
     <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B4:L5"/>
-    <mergeCell ref="B6:L6"/>
-    <mergeCell ref="B14:L15"/>
-    <mergeCell ref="B16:L16"/>
-    <mergeCell ref="B25:L26"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3580,1771 +3801,1468 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C018806-64C8-4635-AE41-CA39982E874B}">
-  <dimension ref="A1:M143"/>
+  <dimension ref="B1:L43"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="D2" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11">
+    <row r="3" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
         <v>3</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="11" t="s">
+      <c r="F3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="K2" s="16">
+      <c r="L3" s="16">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+    <row r="4" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="K3" s="14">
+      <c r="L4" s="14">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+    <row r="5" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="15">
         <v>3</v>
       </c>
-      <c r="B4" s="11">
+      <c r="C5" s="11">
         <v>4</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="11" t="s">
+      <c r="F5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="H5" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="K4" s="16">
+      <c r="L5" s="16">
         <v>37</v>
       </c>
-      <c r="M4" s="39"/>
-    </row>
-    <row r="5" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+    </row>
+    <row r="6" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="K5" s="14">
+      <c r="L6" s="14">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+    <row r="7" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="11">
+      <c r="C7" s="11">
         <v>3</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="F7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="K6" s="16">
+      <c r="L7" s="16">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+    <row r="8" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C8" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="K7" s="14">
+      <c r="L8" s="14">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+    <row r="9" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B9" s="15">
         <v>7</v>
       </c>
-      <c r="B8" s="11">
+      <c r="C9" s="11">
         <v>5</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="E9" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="11" t="s">
+      <c r="F9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="H9" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K8" s="16">
+      <c r="L9" s="16">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+    <row r="10" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C10" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="K9" s="14">
+      <c r="L10" s="14">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+    <row r="11" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B11" s="15">
         <v>9</v>
       </c>
-      <c r="B10" s="11">
+      <c r="C11" s="11">
         <v>5</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="F11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="H11" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="I11" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="K10" s="16">
+      <c r="L11" s="16">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
+    <row r="12" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B12" s="13">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
         <v>4</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K11" s="14">
+      <c r="L12" s="14">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+    <row r="13" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B13" s="15">
         <v>11</v>
       </c>
-      <c r="B12" s="11">
+      <c r="C13" s="11">
         <v>5</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="E13" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="11" t="s">
+      <c r="F13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="H13" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="I13" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="K12" s="16">
+      <c r="L13" s="16">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+    <row r="14" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="13">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C14" s="1">
         <v>2</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="F14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="K14" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="14">
+      <c r="L14" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+    <row r="15" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="15">
         <v>13</v>
       </c>
-      <c r="B14" s="11">
-        <v>1</v>
-      </c>
-      <c r="C14" s="11">
-        <v>10</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="11" t="s">
+      <c r="C15" s="11">
+        <v>1</v>
+      </c>
+      <c r="D15" s="11">
+        <v>10</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="H15" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="I15" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K14" s="16">
+      <c r="L15" s="16">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+    <row r="16" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B16" s="13">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C16" s="1">
         <v>3</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="F16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="K15" s="14">
+      <c r="L16" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
+    <row r="17" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="15">
         <v>15</v>
       </c>
-      <c r="B16" s="11">
-        <v>1</v>
-      </c>
-      <c r="C16" s="11">
-        <v>10</v>
-      </c>
-      <c r="D16" s="11" t="s">
+      <c r="C17" s="11">
+        <v>1</v>
+      </c>
+      <c r="D17" s="11">
+        <v>10</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="11" t="s">
+      <c r="F17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="H17" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="K16" s="16">
+      <c r="L17" s="16">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+    <row r="18" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B18" s="13">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="C18" s="1">
         <v>4</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="K18" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="14">
+      <c r="L18" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
+    <row r="19" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="15">
         <v>17</v>
       </c>
-      <c r="B18" s="11">
-        <v>1</v>
-      </c>
-      <c r="C18" s="11">
-        <v>10</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="11" t="s">
+      <c r="C19" s="11">
+        <v>1</v>
+      </c>
+      <c r="D19" s="11">
+        <v>10</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="I19" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K18" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
+      <c r="L19" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B20" s="13">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C20" s="1">
         <v>3</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="K20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="K19" s="14">
+      <c r="L20" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+    <row r="21" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="15">
         <v>19</v>
       </c>
-      <c r="B20" s="11">
+      <c r="C21" s="11">
         <v>2</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="11" t="s">
+      <c r="F21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="I21" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="16">
+      <c r="L21" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
+    <row r="22" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="13">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1">
-        <v>10</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="K22" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="K21" s="14">
+      <c r="L22" s="14">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
+    <row r="23" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="15">
         <v>21</v>
       </c>
-      <c r="B22" s="11">
-        <v>1</v>
-      </c>
-      <c r="C22" s="11">
-        <v>10</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="11" t="s">
+      <c r="C23" s="11">
+        <v>1</v>
+      </c>
+      <c r="D23" s="11">
+        <v>10</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="G23" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="H23" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="I23" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K22" s="16">
+      <c r="L23" s="16">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
+    <row r="24" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="13">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1">
-        <v>10</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="J24" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="K24" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="K23" s="14">
+      <c r="L24" s="14">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+    <row r="25" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="15">
         <v>23</v>
       </c>
-      <c r="B24" s="11">
-        <v>1</v>
-      </c>
-      <c r="C24" s="11">
-        <v>10</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="11" t="s">
+      <c r="C25" s="11">
+        <v>1</v>
+      </c>
+      <c r="D25" s="11">
+        <v>10</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="H25" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="I25" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="K25" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K24" s="16">
+      <c r="L25" s="16">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
+    <row r="26" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="13">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1">
-        <v>10</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="K26" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="K25" s="14">
+      <c r="L26" s="14">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+    <row r="27" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="15">
         <v>25</v>
       </c>
-      <c r="B26" s="11">
-        <v>1</v>
-      </c>
-      <c r="C26" s="11">
-        <v>10</v>
-      </c>
-      <c r="D26" s="11" t="s">
+      <c r="C27" s="11">
+        <v>1</v>
+      </c>
+      <c r="D27" s="11">
+        <v>10</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="11" t="s">
+      <c r="F27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="H27" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="I27" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="K26" s="16">
+      <c r="L27" s="16">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="1">
-        <v>10</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="1" t="s">
+    <row r="28" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="13">
+        <v>26</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="K28" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="K27" s="14">
+      <c r="L28" s="14">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+    <row r="29" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="15">
         <v>27</v>
       </c>
-      <c r="B28" s="11">
-        <v>1</v>
-      </c>
-      <c r="C28" s="11">
-        <v>10</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="11" t="s">
+      <c r="C29" s="11">
+        <v>1</v>
+      </c>
+      <c r="D29" s="11">
+        <v>10</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="G29" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="H29" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="I29" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="J29" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="K29" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="K28" s="16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
+      <c r="L29" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B30" s="13">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="J30" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="K30" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="K29" s="14">
+      <c r="L30" s="14">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
+    <row r="31" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B31" s="15">
         <v>29</v>
       </c>
-      <c r="B30" s="11">
-        <v>1</v>
-      </c>
-      <c r="C30" s="11">
-        <v>10</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="11" t="s">
+      <c r="C31" s="11">
+        <v>1</v>
+      </c>
+      <c r="D31" s="11">
+        <v>10</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="H31" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="I31" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="K31" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="K30" s="16">
+      <c r="L31" s="16">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13">
+    <row r="32" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B32" s="13">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="1">
-        <v>10</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" s="1" t="s">
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>10</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="K32" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="K31" s="14">
+      <c r="L32" s="14">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
+    <row r="33" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B33" s="15">
         <v>31</v>
       </c>
-      <c r="B32" s="11">
-        <v>1</v>
-      </c>
-      <c r="C32" s="11">
-        <v>10</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="11" t="s">
+      <c r="C33" s="11">
+        <v>1</v>
+      </c>
+      <c r="D33" s="11">
+        <v>10</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="G33" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="H33" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="I33" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="J33" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="K33" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K32" s="16">
+      <c r="L33" s="16">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="13">
+    <row r="34" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B34" s="13">
         <v>32</v>
       </c>
-      <c r="B33" s="1">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1">
-        <v>10</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33" s="1" t="s">
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>10</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="J34" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="K34" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="K33" s="14">
+      <c r="L34" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+    <row r="35" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="15">
         <v>33</v>
       </c>
-      <c r="B34" s="11">
-        <v>1</v>
-      </c>
-      <c r="C34" s="11">
-        <v>10</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" s="11" t="s">
+      <c r="C35" s="11">
+        <v>1</v>
+      </c>
+      <c r="D35" s="11">
+        <v>10</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="H35" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="H34" s="11" t="s">
+      <c r="I35" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="J35" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="K35" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="K34" s="16">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="13">
+      <c r="L35" s="16">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B36" s="13">
         <v>34</v>
       </c>
-      <c r="B35" s="1">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1">
-        <v>10</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
+        <v>10</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" s="1" t="s">
+      <c r="F36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="J36" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="J35" s="3" t="s">
+      <c r="K36" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="K35" s="14">
+      <c r="L36" s="14">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
+    <row r="37" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B37" s="15">
         <v>35</v>
       </c>
-      <c r="B36" s="11">
-        <v>1</v>
-      </c>
-      <c r="C36" s="11">
-        <v>10</v>
-      </c>
-      <c r="D36" s="11" t="s">
+      <c r="C37" s="11">
+        <v>1</v>
+      </c>
+      <c r="D37" s="11">
+        <v>10</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" s="11" t="s">
+      <c r="F37" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="H37" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="H36" s="11" t="s">
+      <c r="I37" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="J37" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="K37" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="K36" s="16">
+      <c r="L37" s="16">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="13">
+    <row r="38" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B38" s="13">
         <v>36</v>
       </c>
-      <c r="B37" s="1">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1">
-        <v>10</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>10</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F37" s="1" t="s">
+      <c r="F38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I37" s="3" t="s">
+      <c r="J38" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="J37" s="3" t="s">
+      <c r="K38" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="K37" s="14">
+      <c r="L38" s="14">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
+    <row r="39" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B39" s="15">
         <v>37</v>
       </c>
-      <c r="B38" s="11">
-        <v>1</v>
-      </c>
-      <c r="C38" s="11">
-        <v>10</v>
-      </c>
-      <c r="D38" s="11" t="s">
+      <c r="C39" s="11">
+        <v>1</v>
+      </c>
+      <c r="D39" s="11">
+        <v>10</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" s="11" t="s">
+      <c r="F39" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="H39" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="H38" s="11" t="s">
+      <c r="I39" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="J39" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="K39" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="K38" s="16">
+      <c r="L39" s="16">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13">
+    <row r="40" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B40" s="13">
         <v>38</v>
       </c>
-      <c r="B39" s="1">
-        <v>1</v>
-      </c>
-      <c r="C39" s="1">
-        <v>10</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>10</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" s="1" t="s">
+      <c r="F40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="I39" s="3" t="s">
+      <c r="J40" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="J39" s="3" t="s">
+      <c r="K40" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="K39" s="14">
+      <c r="L40" s="14">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="15">
+    <row r="41" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B41" s="15">
         <v>39</v>
       </c>
-      <c r="B40" s="11">
-        <v>1</v>
-      </c>
-      <c r="C40" s="11">
-        <v>10</v>
-      </c>
-      <c r="D40" s="11" t="s">
+      <c r="C41" s="11">
+        <v>1</v>
+      </c>
+      <c r="D41" s="11">
+        <v>10</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E40" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F40" s="11" t="s">
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G41" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="H41" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="H40" s="11" t="s">
+      <c r="I41" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="J41" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="K41" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="K40" s="16">
+      <c r="L41" s="16">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="17">
+    <row r="42" spans="2:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="17">
         <v>40</v>
       </c>
-      <c r="B41" s="18">
-        <v>1</v>
-      </c>
-      <c r="C41" s="18">
-        <v>10</v>
-      </c>
-      <c r="D41" s="18" t="s">
+      <c r="C42" s="18">
+        <v>1</v>
+      </c>
+      <c r="D42" s="18">
+        <v>10</v>
+      </c>
+      <c r="E42" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E41" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" s="18" t="s">
+      <c r="F42" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="G41" s="18" t="s">
+      <c r="H42" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="H41" s="18" t="s">
+      <c r="I42" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="I41" s="19" t="s">
+      <c r="J42" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="J41" s="19" t="s">
+      <c r="K42" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="K41" s="20">
+      <c r="L42" s="20">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J42" s="40"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J43" s="39"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J44" s="39"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J45" s="39"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J46" s="39"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J47" s="39"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J48" s="39"/>
-    </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J49" s="39"/>
-    </row>
-    <row r="50" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J50" s="39"/>
-    </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J51" s="39"/>
-    </row>
-    <row r="52" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J52" s="39"/>
-    </row>
-    <row r="53" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J53" s="39"/>
-    </row>
-    <row r="54" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J54" s="39"/>
-    </row>
-    <row r="55" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J55" s="39"/>
-    </row>
-    <row r="56" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J56" s="39"/>
-    </row>
-    <row r="57" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J57" s="39"/>
-    </row>
-    <row r="58" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J58" s="39"/>
-    </row>
-    <row r="59" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J59" s="39"/>
-    </row>
-    <row r="60" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J60" s="39"/>
-    </row>
-    <row r="61" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J61" s="39"/>
-    </row>
-    <row r="62" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J62" s="39"/>
-    </row>
-    <row r="63" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J63" s="39"/>
-    </row>
-    <row r="64" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J64" s="39"/>
-    </row>
-    <row r="65" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J65" s="39"/>
-    </row>
-    <row r="66" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J66" s="39"/>
-    </row>
-    <row r="67" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J67" s="39"/>
-    </row>
-    <row r="68" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J68" s="39"/>
-    </row>
-    <row r="69" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J69" s="39"/>
-    </row>
-    <row r="70" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J70" s="39"/>
-    </row>
-    <row r="71" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J71" s="39"/>
-    </row>
-    <row r="72" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J72" s="39"/>
-    </row>
-    <row r="73" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J73" s="39"/>
-    </row>
-    <row r="74" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J74" s="39"/>
-    </row>
-    <row r="75" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J75" s="39"/>
-    </row>
-    <row r="76" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J76" s="39"/>
-    </row>
-    <row r="77" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J77" s="39"/>
-    </row>
-    <row r="78" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J78" s="39"/>
-    </row>
-    <row r="79" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J79" s="39"/>
-    </row>
-    <row r="80" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J80" s="39"/>
-    </row>
-    <row r="81" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J81" s="39"/>
-    </row>
-    <row r="82" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J82" s="39"/>
-    </row>
-    <row r="83" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J83" s="39"/>
-    </row>
-    <row r="84" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J84" s="39"/>
-    </row>
-    <row r="85" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J85" s="39"/>
-    </row>
-    <row r="86" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J86" s="39"/>
-    </row>
-    <row r="87" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J87" s="39"/>
-    </row>
-    <row r="88" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J88" s="39"/>
-    </row>
-    <row r="89" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J89" s="39"/>
-    </row>
-    <row r="90" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J90" s="39"/>
-    </row>
-    <row r="91" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J91" s="39"/>
-    </row>
-    <row r="92" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J92" s="39"/>
-    </row>
-    <row r="93" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J93" s="39"/>
-    </row>
-    <row r="94" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J94" s="39"/>
-    </row>
-    <row r="95" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J95" s="39"/>
-    </row>
-    <row r="96" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J96" s="39"/>
-    </row>
-    <row r="97" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J97" s="39"/>
-    </row>
-    <row r="98" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J98" s="39"/>
-    </row>
-    <row r="99" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J99" s="39"/>
-    </row>
-    <row r="100" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J100" s="39"/>
-    </row>
-    <row r="101" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J101" s="39"/>
-    </row>
-    <row r="102" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J102" s="39"/>
-    </row>
-    <row r="103" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J103" s="39"/>
-    </row>
-    <row r="104" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J104" s="39"/>
-    </row>
-    <row r="105" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J105" s="39"/>
-    </row>
-    <row r="106" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J106" s="39"/>
-    </row>
-    <row r="107" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J107" s="39"/>
-    </row>
-    <row r="108" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J108" s="39"/>
-    </row>
-    <row r="109" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J109" s="39"/>
-    </row>
-    <row r="110" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J110" s="39"/>
-    </row>
-    <row r="111" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J111" s="39"/>
-    </row>
-    <row r="112" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J112" s="39"/>
-    </row>
-    <row r="113" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J113" s="39"/>
-    </row>
-    <row r="114" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J114" s="39"/>
-    </row>
-    <row r="115" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J115" s="39"/>
-    </row>
-    <row r="116" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J116" s="39"/>
-    </row>
-    <row r="117" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J117" s="39"/>
-    </row>
-    <row r="118" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J118" s="39"/>
-    </row>
-    <row r="119" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J119" s="39"/>
-    </row>
-    <row r="120" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J120" s="39"/>
-    </row>
-    <row r="121" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J121" s="39"/>
-    </row>
-    <row r="122" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J122" s="39"/>
-    </row>
-    <row r="123" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J123" s="39"/>
-    </row>
-    <row r="124" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J124" s="39"/>
-    </row>
-    <row r="125" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J125" s="39"/>
-    </row>
-    <row r="126" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J126" s="39"/>
-    </row>
-    <row r="127" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J127" s="39"/>
-    </row>
-    <row r="128" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J128" s="39"/>
-    </row>
-    <row r="129" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J129" s="39"/>
-    </row>
-    <row r="130" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J130" s="39"/>
-    </row>
-    <row r="131" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J131" s="39"/>
-    </row>
-    <row r="132" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J132" s="39"/>
-    </row>
-    <row r="133" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J133" s="39"/>
-    </row>
-    <row r="134" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J134" s="39"/>
-    </row>
-    <row r="135" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J135" s="39"/>
-    </row>
-    <row r="136" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J136" s="39"/>
-    </row>
-    <row r="137" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J137" s="39"/>
-    </row>
-    <row r="138" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J138" s="39"/>
-    </row>
-    <row r="139" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J139" s="39"/>
-    </row>
-    <row r="140" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J140" s="39"/>
-    </row>
-    <row r="141" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J141" s="39"/>
-    </row>
-    <row r="142" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J142" s="39"/>
-    </row>
-    <row r="143" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J143" s="39"/>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K43" s="36"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K41">
-    <sortCondition descending="1" ref="G2:G41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:L42">
+    <sortCondition descending="1" ref="H3:H42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5352,181 +5270,609 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDB22E6-1706-470A-86D1-C920EAE26AA9}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="B1:M5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.125" customWidth="1"/>
-    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="D2" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H2" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="L2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="M3" s="14" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+    <row r="4" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="D3" s="11">
+      <c r="E4" s="11">
         <v>3</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="11" t="s">
+      <c r="H4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="M4" s="16" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17">
+    <row r="5" spans="2:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="C5" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D5" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="D4" s="18">
+      <c r="E5" s="18">
         <v>4</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="F5" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="G5" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="18" t="s">
+      <c r="H5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="J5" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="K5" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="L5" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="M5" s="20" t="s">
         <v>245</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E78735-6CB7-46FE-9582-770B304E21CE}">
+  <dimension ref="A4:M18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="46"/>
+      <c r="B4" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="48"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="58" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" s="59"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="K4" s="59"/>
+      <c r="L4" s="60"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="46"/>
+      <c r="B5" s="50" t="s">
+        <v>253</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>255</v>
+      </c>
+      <c r="E5" s="40"/>
+      <c r="F5" s="50" t="s">
+        <v>253</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>254</v>
+      </c>
+      <c r="H5" s="52" t="s">
+        <v>255</v>
+      </c>
+      <c r="I5" s="40"/>
+      <c r="J5" s="50" t="s">
+        <v>253</v>
+      </c>
+      <c r="K5" s="51" t="s">
+        <v>254</v>
+      </c>
+      <c r="L5" s="52" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="46"/>
+      <c r="B6" s="40">
+        <v>1</v>
+      </c>
+      <c r="C6" s="40">
+        <v>1</v>
+      </c>
+      <c r="D6" s="42">
+        <v>1</v>
+      </c>
+      <c r="E6" s="40"/>
+      <c r="F6" s="53">
+        <v>1</v>
+      </c>
+      <c r="G6" s="54">
+        <v>1</v>
+      </c>
+      <c r="H6" s="42">
+        <v>1</v>
+      </c>
+      <c r="I6" s="40"/>
+      <c r="J6" s="53">
+        <v>1</v>
+      </c>
+      <c r="K6" s="54">
+        <v>1</v>
+      </c>
+      <c r="L6" s="42">
+        <v>1</v>
+      </c>
+      <c r="M6" s="61"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="46"/>
+      <c r="B7" s="41">
+        <v>1</v>
+      </c>
+      <c r="C7" s="41">
+        <v>1</v>
+      </c>
+      <c r="D7" s="43">
+        <v>1</v>
+      </c>
+      <c r="E7" s="40"/>
+      <c r="F7" s="55">
+        <v>1</v>
+      </c>
+      <c r="G7" s="56">
+        <v>1</v>
+      </c>
+      <c r="H7" s="43">
+        <v>1</v>
+      </c>
+      <c r="I7" s="40"/>
+      <c r="J7" s="55">
+        <v>1</v>
+      </c>
+      <c r="K7" s="56">
+        <v>1</v>
+      </c>
+      <c r="L7" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="46"/>
+      <c r="B8" s="40">
+        <v>0</v>
+      </c>
+      <c r="C8" s="40">
+        <v>1</v>
+      </c>
+      <c r="D8" s="42">
+        <v>0</v>
+      </c>
+      <c r="E8" s="40"/>
+      <c r="F8" s="53">
+        <v>0</v>
+      </c>
+      <c r="G8" s="54">
+        <v>1</v>
+      </c>
+      <c r="H8" s="42">
+        <v>0</v>
+      </c>
+      <c r="I8" s="40"/>
+      <c r="J8" s="53">
+        <v>0</v>
+      </c>
+      <c r="K8" s="54">
+        <v>1</v>
+      </c>
+      <c r="L8" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="46"/>
+      <c r="B9" s="41">
+        <v>1</v>
+      </c>
+      <c r="C9" s="41">
+        <v>1</v>
+      </c>
+      <c r="D9" s="43">
+        <v>1</v>
+      </c>
+      <c r="E9" s="40"/>
+      <c r="F9" s="55">
+        <v>0</v>
+      </c>
+      <c r="G9" s="56">
+        <v>1</v>
+      </c>
+      <c r="H9" s="43">
+        <v>0</v>
+      </c>
+      <c r="I9" s="40"/>
+      <c r="J9" s="55">
+        <v>1</v>
+      </c>
+      <c r="K9" s="56">
+        <v>1</v>
+      </c>
+      <c r="L9" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="46"/>
+      <c r="B10" s="40">
+        <v>0</v>
+      </c>
+      <c r="C10" s="40">
+        <v>1</v>
+      </c>
+      <c r="D10" s="42">
+        <v>0</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="53">
+        <v>0</v>
+      </c>
+      <c r="G10" s="54">
+        <v>1</v>
+      </c>
+      <c r="H10" s="42">
+        <v>0</v>
+      </c>
+      <c r="I10" s="40"/>
+      <c r="J10" s="53">
+        <v>0</v>
+      </c>
+      <c r="K10" s="54">
+        <v>1</v>
+      </c>
+      <c r="L10" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="46"/>
+      <c r="B11" s="41">
+        <v>0</v>
+      </c>
+      <c r="C11" s="41">
+        <v>0</v>
+      </c>
+      <c r="D11" s="43">
+        <v>1</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="55">
+        <v>0</v>
+      </c>
+      <c r="G11" s="56">
+        <v>0</v>
+      </c>
+      <c r="H11" s="43">
+        <v>1</v>
+      </c>
+      <c r="I11" s="40"/>
+      <c r="J11" s="55">
+        <v>0</v>
+      </c>
+      <c r="K11" s="56">
+        <v>0</v>
+      </c>
+      <c r="L11" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="46"/>
+      <c r="B12" s="40">
+        <v>0</v>
+      </c>
+      <c r="C12" s="40">
+        <v>0</v>
+      </c>
+      <c r="D12" s="42">
+        <v>1</v>
+      </c>
+      <c r="E12" s="40"/>
+      <c r="F12" s="53">
+        <v>0</v>
+      </c>
+      <c r="G12" s="54">
+        <v>0</v>
+      </c>
+      <c r="H12" s="42">
+        <v>1</v>
+      </c>
+      <c r="I12" s="40"/>
+      <c r="J12" s="53">
+        <v>0</v>
+      </c>
+      <c r="K12" s="54">
+        <v>0</v>
+      </c>
+      <c r="L12" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="46"/>
+      <c r="B13" s="41">
+        <v>1</v>
+      </c>
+      <c r="C13" s="41">
+        <v>0</v>
+      </c>
+      <c r="D13" s="43">
+        <v>0</v>
+      </c>
+      <c r="E13" s="40"/>
+      <c r="F13" s="55">
+        <v>1</v>
+      </c>
+      <c r="G13" s="56">
+        <v>0</v>
+      </c>
+      <c r="H13" s="43">
+        <v>0</v>
+      </c>
+      <c r="I13" s="40"/>
+      <c r="J13" s="55">
+        <v>1</v>
+      </c>
+      <c r="K13" s="56">
+        <v>0</v>
+      </c>
+      <c r="L13" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="46"/>
+      <c r="B14" s="40">
+        <v>0</v>
+      </c>
+      <c r="C14" s="40">
+        <v>0</v>
+      </c>
+      <c r="D14" s="42">
+        <v>1</v>
+      </c>
+      <c r="E14" s="40"/>
+      <c r="F14" s="53">
+        <v>0</v>
+      </c>
+      <c r="G14" s="54">
+        <v>0</v>
+      </c>
+      <c r="H14" s="42">
+        <v>1</v>
+      </c>
+      <c r="I14" s="40"/>
+      <c r="J14" s="53">
+        <v>0</v>
+      </c>
+      <c r="K14" s="54">
+        <v>0</v>
+      </c>
+      <c r="L14" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="46"/>
+      <c r="B15" s="44">
+        <v>1</v>
+      </c>
+      <c r="C15" s="44">
+        <v>0</v>
+      </c>
+      <c r="D15" s="45">
+        <v>0</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="57">
+        <v>1</v>
+      </c>
+      <c r="G15" s="44">
+        <v>0</v>
+      </c>
+      <c r="H15" s="45">
+        <v>0</v>
+      </c>
+      <c r="I15" s="40"/>
+      <c r="J15" s="57">
+        <v>1</v>
+      </c>
+      <c r="K15" s="44">
+        <v>0</v>
+      </c>
+      <c r="L15" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="63" t="s">
+        <v>256</v>
+      </c>
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
+      <c r="F16" s="63" t="s">
+        <v>257</v>
+      </c>
+      <c r="G16" s="64"/>
+      <c r="H16" s="65"/>
+      <c r="J16" s="63" t="s">
+        <v>256</v>
+      </c>
+      <c r="K16" s="64"/>
+      <c r="L16" s="65"/>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="62"/>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H18" s="66"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B16:D16"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D6:D15 H6:H15 L6:L15">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>